<commit_message>
Updated bulk app translation sheet format to correspond to case list page redesign
</commit_message>
<xml_diff>
--- a/corehq/apps/app_manager/tests/data/bulk_app_translations.xlsx
+++ b/corehq/apps/app_manager/tests/data/bulk_app_translations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25203"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modules_and_forms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>in french</t>
+  </si>
+  <si>
+    <t>list_or_detail</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>detail</t>
   </si>
 </sst>
 </file>
@@ -586,71 +595,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="1" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -668,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add label for cases columns to the first sheet
</commit_message>
<xml_diff>
--- a/corehq/apps/app_manager/tests/data/bulk_app_translations.xlsx
+++ b/corehq/apps/app_manager/tests/data/bulk_app_translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25203"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="25360" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Modules_and_forms" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="54">
   <si>
     <t>Type</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>detail</t>
+  </si>
+  <si>
+    <t>label_for_cases_en</t>
+  </si>
+  <si>
+    <t>label_for_cases_fra</t>
+  </si>
+  <si>
+    <t>Cases</t>
   </si>
 </sst>
 </file>
@@ -505,16 +514,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,16 +541,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -551,16 +570,22 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -573,13 +598,13 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -597,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>